<commit_message>
BugFix: Conflito de nome de intervalos
</commit_message>
<xml_diff>
--- a/Forms/Form_161_maior.xlsx
+++ b/Forms/Form_161_maior.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levym\OneDrive\Documentos\Projects\Tecplas\Sis-Pint\projeto_pintura\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6CE2C9-505A-4D21-871D-03A16FECF8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB92864D-B2AE-460C-9873-9F6F53C36937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="F966" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -20,9 +20,6 @@
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase" localSheetId="1" hidden="1">Dados!$A$1:$L$69</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilha1!$A$1:$K$102</definedName>
-    <definedName name="Print_Area" localSheetId="2">'40-157'!$B$1:$L$59</definedName>
-    <definedName name="Print_Area" localSheetId="0">Planilha1!$A$1:$K$102</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1771,119 +1768,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1941,6 +1889,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1950,65 +1904,158 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2031,17 +2078,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2049,64 +2090,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -22118,67 +22115,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="109" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="129"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="111"/>
     </row>
     <row r="2" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="130"/>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131"/>
-      <c r="K2" s="132"/>
+      <c r="A2" s="112"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="114"/>
     </row>
     <row r="3" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="135" t="s">
+      <c r="A3" s="117" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="136"/>
-      <c r="C3" s="138" t="s">
+      <c r="B3" s="118"/>
+      <c r="C3" s="120" t="s">
         <v>231</v>
       </c>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="133">
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="115">
         <v>116897</v>
       </c>
-      <c r="K3" s="134"/>
+      <c r="K3" s="116"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="135" t="s">
+      <c r="A4" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="136"/>
-      <c r="C4" s="139" t="s">
+      <c r="B4" s="118"/>
+      <c r="C4" s="121" t="s">
         <v>232</v>
       </c>
-      <c r="D4" s="139"/>
-      <c r="E4" s="139"/>
-      <c r="F4" s="140"/>
-      <c r="G4" s="141" t="s">
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="142"/>
+      <c r="H4" s="124"/>
       <c r="I4" s="82">
         <v>44963</v>
       </c>
@@ -22193,60 +22190,60 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="112" t="s">
+      <c r="A6" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
+      <c r="B6" s="125"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="125"/>
+      <c r="J6" s="125"/>
+      <c r="K6" s="125"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="112"/>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
+      <c r="A7" s="125"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="125"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="125"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="102" t="s">
+      <c r="A8" s="161" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="102"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="102"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="92" t="s">
+      <c r="B8" s="161"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="161"/>
+      <c r="E8" s="161"/>
+      <c r="F8" s="161"/>
+      <c r="G8" s="161"/>
+      <c r="H8" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92" t="s">
+      <c r="I8" s="96"/>
+      <c r="J8" s="96" t="s">
         <v>123</v>
       </c>
-      <c r="K8" s="92"/>
+      <c r="K8" s="96"/>
     </row>
     <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="102"/>
-      <c r="B9" s="102"/>
-      <c r="C9" s="102"/>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
+      <c r="A9" s="161"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="161"/>
+      <c r="F9" s="161"/>
+      <c r="G9" s="161"/>
       <c r="H9" s="4" t="s">
         <v>18</v>
       </c>
@@ -22257,13 +22254,13 @@
       <c r="K9" s="80"/>
     </row>
     <row r="10" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="102"/>
-      <c r="B10" s="102"/>
-      <c r="C10" s="102"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
+      <c r="A10" s="161"/>
+      <c r="B10" s="161"/>
+      <c r="C10" s="161"/>
+      <c r="D10" s="161"/>
+      <c r="E10" s="161"/>
+      <c r="F10" s="161"/>
+      <c r="G10" s="161"/>
       <c r="H10" s="4" t="s">
         <v>17</v>
       </c>
@@ -22274,13 +22271,13 @@
       <c r="K10" s="80"/>
     </row>
     <row r="11" spans="1:11" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="102"/>
-      <c r="B11" s="102"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
+      <c r="A11" s="161"/>
+      <c r="B11" s="161"/>
+      <c r="C11" s="161"/>
+      <c r="D11" s="161"/>
+      <c r="E11" s="161"/>
+      <c r="F11" s="161"/>
+      <c r="G11" s="161"/>
       <c r="H11" s="4" t="s">
         <v>106</v>
       </c>
@@ -22295,13 +22292,13 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="102"/>
-      <c r="B12" s="102"/>
-      <c r="C12" s="102"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="102"/>
-      <c r="G12" s="102"/>
+      <c r="A12" s="161"/>
+      <c r="B12" s="161"/>
+      <c r="C12" s="161"/>
+      <c r="D12" s="161"/>
+      <c r="E12" s="161"/>
+      <c r="F12" s="161"/>
+      <c r="G12" s="161"/>
       <c r="H12" s="4" t="s">
         <v>107</v>
       </c>
@@ -22329,50 +22326,50 @@
       <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="154" t="s">
         <v>110</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="96" t="str">
+      <c r="B14" s="155"/>
+      <c r="C14" s="155"/>
+      <c r="D14" s="156"/>
+      <c r="E14" s="130" t="str">
         <f>VLOOKUP(J3,Dados!A:H,5,0)</f>
         <v>&lt;=45 psi</v>
       </c>
-      <c r="F14" s="97"/>
-      <c r="G14" s="98"/>
-      <c r="H14" s="103" t="s">
+      <c r="F14" s="157"/>
+      <c r="G14" s="131"/>
+      <c r="H14" s="126" t="s">
         <v>121</v>
       </c>
-      <c r="I14" s="103"/>
-      <c r="J14" s="103" t="s">
+      <c r="I14" s="126"/>
+      <c r="J14" s="126" t="s">
         <v>122</v>
       </c>
-      <c r="K14" s="103"/>
+      <c r="K14" s="126"/>
     </row>
     <row r="15" spans="1:11" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="93" t="s">
+      <c r="A15" s="154" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="94"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="94"/>
-      <c r="G15" s="94"/>
-      <c r="H15" s="94"/>
-      <c r="I15" s="94"/>
-      <c r="J15" s="94"/>
-      <c r="K15" s="95"/>
+      <c r="B15" s="155"/>
+      <c r="C15" s="155"/>
+      <c r="D15" s="155"/>
+      <c r="E15" s="155"/>
+      <c r="F15" s="155"/>
+      <c r="G15" s="155"/>
+      <c r="H15" s="155"/>
+      <c r="I15" s="155"/>
+      <c r="J15" s="155"/>
+      <c r="K15" s="156"/>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="99"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="100"/>
-      <c r="F16" s="100"/>
-      <c r="G16" s="101"/>
+      <c r="A16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="160"/>
       <c r="H16" s="26" t="s">
         <v>2</v>
       </c>
@@ -22387,15 +22384,15 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="143"/>
-      <c r="B17" s="144"/>
-      <c r="C17" s="144"/>
-      <c r="D17" s="144"/>
-      <c r="E17" s="145"/>
-      <c r="F17" s="126" t="s">
+      <c r="A17" s="127"/>
+      <c r="B17" s="128"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="128"/>
+      <c r="E17" s="129"/>
+      <c r="F17" s="108" t="s">
         <v>125</v>
       </c>
-      <c r="G17" s="126"/>
+      <c r="G17" s="108"/>
       <c r="H17" s="29" t="str">
         <f>VLOOKUP(J3,Dados!A:N,14,0)</f>
         <v>___:____</v>
@@ -22417,22 +22414,22 @@
       <c r="A18" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="B18" s="96" t="str">
+      <c r="B18" s="130" t="str">
         <f>VLOOKUP(J3,Dados!A:W,23,0)</f>
         <v>1.8 a 2mm</v>
       </c>
-      <c r="C18" s="98"/>
-      <c r="D18" s="155" t="s">
+      <c r="C18" s="131"/>
+      <c r="D18" s="99" t="s">
         <v>147</v>
       </c>
-      <c r="E18" s="155" t="str">
+      <c r="E18" s="99" t="str">
         <f>VLOOKUP(J3,Dados!A:M,13,0)</f>
         <v>30 Min./ Mínimo</v>
       </c>
-      <c r="F18" s="92" t="s">
+      <c r="F18" s="96" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="92"/>
+      <c r="G18" s="96"/>
       <c r="H18" s="2" t="str">
         <f>VLOOKUP(J3,Dados!A:P,16,0)</f>
         <v>___:____</v>
@@ -22451,20 +22448,20 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="153" t="s">
+      <c r="A19" s="97" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="92">
+      <c r="B19" s="96">
         <f>VLOOKUP(J3,Dados!A:L,12,0)</f>
         <v>2</v>
       </c>
-      <c r="C19" s="92"/>
-      <c r="D19" s="156"/>
-      <c r="E19" s="156"/>
-      <c r="F19" s="92" t="s">
+      <c r="C19" s="96"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="96" t="s">
         <v>228</v>
       </c>
-      <c r="G19" s="92"/>
+      <c r="G19" s="96"/>
       <c r="H19" s="2" t="str">
         <f>VLOOKUP(J3,Dados!A:R,18,0)</f>
         <v>N/A</v>
@@ -22483,15 +22480,15 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="154"/>
-      <c r="B20" s="152"/>
-      <c r="C20" s="152"/>
-      <c r="D20" s="157"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="152" t="s">
+      <c r="A20" s="98"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="101"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="95" t="s">
         <v>133</v>
       </c>
-      <c r="G20" s="152"/>
+      <c r="G20" s="95"/>
       <c r="H20" s="32" t="str">
         <f>VLOOKUP(J3,Dados!A:T,20,0)</f>
         <v>N/A</v>
@@ -22510,139 +22507,139 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="105" t="s">
+      <c r="A21" s="163" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="106"/>
-      <c r="C21" s="106"/>
-      <c r="D21" s="106"/>
-      <c r="E21" s="97" t="str">
+      <c r="B21" s="164"/>
+      <c r="C21" s="164"/>
+      <c r="D21" s="164"/>
+      <c r="E21" s="157" t="str">
         <f>VLOOKUP(J3,Dados!A1:F75,6,0)</f>
         <v>60 min./ Mínimo</v>
       </c>
-      <c r="F21" s="97"/>
-      <c r="G21" s="98"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="131"/>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
       <c r="J21" s="27"/>
       <c r="K21" s="28"/>
     </row>
     <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="93" t="s">
+      <c r="A22" s="154" t="s">
         <v>112</v>
       </c>
-      <c r="B22" s="94"/>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="97" t="str">
+      <c r="B22" s="155"/>
+      <c r="C22" s="155"/>
+      <c r="D22" s="155"/>
+      <c r="E22" s="157" t="str">
         <f>VLOOKUP(J3,Dados!A:H,8,0)</f>
         <v>120 min./ Mínimo</v>
       </c>
-      <c r="F22" s="97"/>
-      <c r="G22" s="98"/>
+      <c r="F22" s="157"/>
+      <c r="G22" s="131"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="93" t="s">
+      <c r="A23" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="97" t="str">
+      <c r="B23" s="155"/>
+      <c r="C23" s="155"/>
+      <c r="D23" s="155"/>
+      <c r="E23" s="157" t="str">
         <f>VLOOKUP(J3,Dados!A:H,7,0)</f>
         <v>58 ± 2° ºC</v>
       </c>
-      <c r="F23" s="97"/>
-      <c r="G23" s="98"/>
-      <c r="H23" s="107"/>
-      <c r="I23" s="107"/>
-      <c r="J23" s="91"/>
-      <c r="K23" s="91"/>
+      <c r="F23" s="157"/>
+      <c r="G23" s="131"/>
+      <c r="H23" s="132"/>
+      <c r="I23" s="132"/>
+      <c r="J23" s="153"/>
+      <c r="K23" s="153"/>
     </row>
     <row r="24" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="108" t="s">
+      <c r="A25" s="133" t="s">
         <v>119</v>
       </c>
-      <c r="B25" s="109"/>
-      <c r="C25" s="109"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="109"/>
-      <c r="G25" s="109"/>
-      <c r="H25" s="109"/>
-      <c r="I25" s="109"/>
-      <c r="J25" s="109"/>
-      <c r="K25" s="110"/>
+      <c r="B25" s="134"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134"/>
+      <c r="F25" s="134"/>
+      <c r="G25" s="134"/>
+      <c r="H25" s="134"/>
+      <c r="I25" s="134"/>
+      <c r="J25" s="134"/>
+      <c r="K25" s="135"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="111"/>
-      <c r="B26" s="112"/>
-      <c r="C26" s="112"/>
-      <c r="D26" s="112"/>
-      <c r="E26" s="112"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="112"/>
-      <c r="H26" s="112"/>
-      <c r="I26" s="112"/>
-      <c r="J26" s="112"/>
-      <c r="K26" s="113"/>
+      <c r="A26" s="136"/>
+      <c r="B26" s="125"/>
+      <c r="C26" s="125"/>
+      <c r="D26" s="125"/>
+      <c r="E26" s="125"/>
+      <c r="F26" s="125"/>
+      <c r="G26" s="125"/>
+      <c r="H26" s="125"/>
+      <c r="I26" s="125"/>
+      <c r="J26" s="125"/>
+      <c r="K26" s="137"/>
     </row>
     <row r="27" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="117" t="s">
+      <c r="A27" s="141" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="118"/>
-      <c r="C27" s="118"/>
-      <c r="D27" s="118"/>
-      <c r="E27" s="118"/>
-      <c r="F27" s="118"/>
-      <c r="G27" s="118"/>
-      <c r="H27" s="118" t="s">
+      <c r="B27" s="142"/>
+      <c r="C27" s="142"/>
+      <c r="D27" s="142"/>
+      <c r="E27" s="142"/>
+      <c r="F27" s="142"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="142" t="s">
         <v>117</v>
       </c>
-      <c r="I27" s="118"/>
-      <c r="J27" s="118"/>
-      <c r="K27" s="119"/>
+      <c r="I27" s="142"/>
+      <c r="J27" s="142"/>
+      <c r="K27" s="143"/>
     </row>
     <row r="28" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="114" t="s">
+      <c r="A28" s="138" t="s">
         <v>116</v>
       </c>
-      <c r="B28" s="115"/>
-      <c r="C28" s="115"/>
-      <c r="D28" s="115"/>
-      <c r="E28" s="115"/>
-      <c r="F28" s="115"/>
-      <c r="G28" s="115"/>
-      <c r="H28" s="115" t="s">
+      <c r="B28" s="139"/>
+      <c r="C28" s="139"/>
+      <c r="D28" s="139"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="139"/>
+      <c r="G28" s="139"/>
+      <c r="H28" s="139" t="s">
         <v>186</v>
       </c>
-      <c r="I28" s="115"/>
-      <c r="J28" s="115"/>
-      <c r="K28" s="116"/>
+      <c r="I28" s="139"/>
+      <c r="J28" s="139"/>
+      <c r="K28" s="140"/>
     </row>
     <row r="29" spans="1:11" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
     </row>
     <row r="30" spans="1:11" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="120" t="s">
+      <c r="A30" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="121"/>
-      <c r="C30" s="121"/>
-      <c r="D30" s="121"/>
-      <c r="E30" s="121"/>
-      <c r="F30" s="121"/>
-      <c r="G30" s="121"/>
-      <c r="H30" s="121"/>
-      <c r="I30" s="121"/>
-      <c r="J30" s="121"/>
-      <c r="K30" s="122"/>
+      <c r="B30" s="145"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
+      <c r="H30" s="145"/>
+      <c r="I30" s="145"/>
+      <c r="J30" s="145"/>
+      <c r="K30" s="146"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -22650,16 +22647,16 @@
       </c>
     </row>
     <row r="33" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="123" t="s">
+      <c r="A33" s="147" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="124"/>
-      <c r="C33" s="124"/>
-      <c r="D33" s="124"/>
-      <c r="E33" s="125"/>
-      <c r="F33" s="104"/>
-      <c r="G33" s="104"/>
-      <c r="H33" s="104"/>
+      <c r="B33" s="148"/>
+      <c r="C33" s="148"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="149"/>
+      <c r="F33" s="162"/>
+      <c r="G33" s="162"/>
+      <c r="H33" s="162"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9" t="s">
         <v>12</v>
@@ -22670,19 +22667,19 @@
     </row>
     <row r="34" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="88">
+      <c r="A35" s="150">
         <v>1</v>
       </c>
-      <c r="B35" s="89"/>
-      <c r="C35" s="89"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="90"/>
-      <c r="F35" s="192">
+      <c r="B35" s="151"/>
+      <c r="C35" s="151"/>
+      <c r="D35" s="151"/>
+      <c r="E35" s="152"/>
+      <c r="F35" s="102">
         <v>90529191900010</v>
       </c>
-      <c r="G35" s="193"/>
-      <c r="H35" s="194"/>
-      <c r="I35" s="195">
+      <c r="G35" s="103"/>
+      <c r="H35" s="104"/>
+      <c r="I35" s="88">
         <v>5</v>
       </c>
       <c r="J35" s="8" t="s">
@@ -22691,19 +22688,19 @@
       <c r="K35" s="5"/>
     </row>
     <row r="36" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="88">
+      <c r="A36" s="150">
         <v>2</v>
       </c>
-      <c r="B36" s="89"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="90"/>
-      <c r="F36" s="192">
+      <c r="B36" s="151"/>
+      <c r="C36" s="151"/>
+      <c r="D36" s="151"/>
+      <c r="E36" s="152"/>
+      <c r="F36" s="102">
         <v>90528218800050</v>
       </c>
-      <c r="G36" s="193"/>
-      <c r="H36" s="194"/>
-      <c r="I36" s="195">
+      <c r="G36" s="103"/>
+      <c r="H36" s="104"/>
+      <c r="I36" s="88">
         <v>10</v>
       </c>
       <c r="J36" s="8" t="s">
@@ -22712,1020 +22709,1020 @@
       <c r="K36" s="5"/>
     </row>
     <row r="37" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="88">
+      <c r="A37" s="150">
         <v>3</v>
       </c>
-      <c r="B37" s="89"/>
-      <c r="C37" s="89"/>
-      <c r="D37" s="89"/>
-      <c r="E37" s="90"/>
-      <c r="F37" s="192"/>
-      <c r="G37" s="193"/>
-      <c r="H37" s="194"/>
-      <c r="I37" s="195"/>
+      <c r="B37" s="151"/>
+      <c r="C37" s="151"/>
+      <c r="D37" s="151"/>
+      <c r="E37" s="152"/>
+      <c r="F37" s="102"/>
+      <c r="G37" s="103"/>
+      <c r="H37" s="104"/>
+      <c r="I37" s="88"/>
       <c r="J37" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K37" s="5"/>
     </row>
     <row r="38" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="88">
+      <c r="A38" s="150">
         <v>4</v>
       </c>
-      <c r="B38" s="89"/>
-      <c r="C38" s="89"/>
-      <c r="D38" s="89"/>
-      <c r="E38" s="90"/>
-      <c r="F38" s="192"/>
-      <c r="G38" s="193"/>
-      <c r="H38" s="194"/>
-      <c r="I38" s="195"/>
+      <c r="B38" s="151"/>
+      <c r="C38" s="151"/>
+      <c r="D38" s="151"/>
+      <c r="E38" s="152"/>
+      <c r="F38" s="102"/>
+      <c r="G38" s="103"/>
+      <c r="H38" s="104"/>
+      <c r="I38" s="88"/>
       <c r="J38" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K38" s="5"/>
     </row>
     <row r="39" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="88">
+      <c r="A39" s="150">
         <v>5</v>
       </c>
-      <c r="B39" s="89"/>
-      <c r="C39" s="89"/>
-      <c r="D39" s="89"/>
-      <c r="E39" s="90"/>
-      <c r="F39" s="192"/>
-      <c r="G39" s="193"/>
-      <c r="H39" s="194"/>
-      <c r="I39" s="195"/>
+      <c r="B39" s="151"/>
+      <c r="C39" s="151"/>
+      <c r="D39" s="151"/>
+      <c r="E39" s="152"/>
+      <c r="F39" s="102"/>
+      <c r="G39" s="103"/>
+      <c r="H39" s="104"/>
+      <c r="I39" s="88"/>
       <c r="J39" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K39" s="5"/>
     </row>
     <row r="40" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="88">
+      <c r="A40" s="150">
         <v>6</v>
       </c>
-      <c r="B40" s="89"/>
-      <c r="C40" s="89"/>
-      <c r="D40" s="89"/>
-      <c r="E40" s="90"/>
-      <c r="F40" s="192"/>
-      <c r="G40" s="193"/>
-      <c r="H40" s="194"/>
-      <c r="I40" s="195"/>
+      <c r="B40" s="151"/>
+      <c r="C40" s="151"/>
+      <c r="D40" s="151"/>
+      <c r="E40" s="152"/>
+      <c r="F40" s="102"/>
+      <c r="G40" s="103"/>
+      <c r="H40" s="104"/>
+      <c r="I40" s="88"/>
       <c r="J40" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="88">
+      <c r="A41" s="150">
         <v>7</v>
       </c>
-      <c r="B41" s="89"/>
-      <c r="C41" s="89"/>
-      <c r="D41" s="89"/>
-      <c r="E41" s="90"/>
-      <c r="F41" s="192"/>
-      <c r="G41" s="193"/>
-      <c r="H41" s="194"/>
-      <c r="I41" s="195"/>
+      <c r="B41" s="151"/>
+      <c r="C41" s="151"/>
+      <c r="D41" s="151"/>
+      <c r="E41" s="152"/>
+      <c r="F41" s="102"/>
+      <c r="G41" s="103"/>
+      <c r="H41" s="104"/>
+      <c r="I41" s="88"/>
       <c r="J41" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K41" s="5"/>
     </row>
     <row r="42" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="88">
+      <c r="A42" s="150">
         <v>8</v>
       </c>
-      <c r="B42" s="89"/>
-      <c r="C42" s="89"/>
-      <c r="D42" s="89"/>
-      <c r="E42" s="90"/>
-      <c r="F42" s="192"/>
-      <c r="G42" s="193"/>
-      <c r="H42" s="194"/>
-      <c r="I42" s="195"/>
+      <c r="B42" s="151"/>
+      <c r="C42" s="151"/>
+      <c r="D42" s="151"/>
+      <c r="E42" s="152"/>
+      <c r="F42" s="102"/>
+      <c r="G42" s="103"/>
+      <c r="H42" s="104"/>
+      <c r="I42" s="88"/>
       <c r="J42" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="88">
+      <c r="A43" s="150">
         <v>9</v>
       </c>
-      <c r="B43" s="89"/>
-      <c r="C43" s="89"/>
-      <c r="D43" s="89"/>
-      <c r="E43" s="90"/>
-      <c r="F43" s="192"/>
-      <c r="G43" s="193"/>
-      <c r="H43" s="194"/>
-      <c r="I43" s="195"/>
+      <c r="B43" s="151"/>
+      <c r="C43" s="151"/>
+      <c r="D43" s="151"/>
+      <c r="E43" s="152"/>
+      <c r="F43" s="102"/>
+      <c r="G43" s="103"/>
+      <c r="H43" s="104"/>
+      <c r="I43" s="88"/>
       <c r="J43" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K43" s="5"/>
     </row>
     <row r="44" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="88">
+      <c r="A44" s="150">
         <v>10</v>
       </c>
-      <c r="B44" s="89"/>
-      <c r="C44" s="89"/>
-      <c r="D44" s="89"/>
-      <c r="E44" s="90"/>
-      <c r="F44" s="192"/>
-      <c r="G44" s="193"/>
-      <c r="H44" s="194"/>
-      <c r="I44" s="195"/>
+      <c r="B44" s="151"/>
+      <c r="C44" s="151"/>
+      <c r="D44" s="151"/>
+      <c r="E44" s="152"/>
+      <c r="F44" s="102"/>
+      <c r="G44" s="103"/>
+      <c r="H44" s="104"/>
+      <c r="I44" s="88"/>
       <c r="J44" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K44" s="5"/>
     </row>
     <row r="45" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="88">
+      <c r="A45" s="150">
         <v>11</v>
       </c>
-      <c r="B45" s="89"/>
-      <c r="C45" s="89"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="192"/>
-      <c r="G45" s="193"/>
-      <c r="H45" s="194"/>
-      <c r="I45" s="195"/>
+      <c r="B45" s="151"/>
+      <c r="C45" s="151"/>
+      <c r="D45" s="151"/>
+      <c r="E45" s="152"/>
+      <c r="F45" s="102"/>
+      <c r="G45" s="103"/>
+      <c r="H45" s="104"/>
+      <c r="I45" s="88"/>
       <c r="J45" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K45" s="5"/>
     </row>
     <row r="46" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="88">
+      <c r="A46" s="150">
         <v>12</v>
       </c>
-      <c r="B46" s="89"/>
-      <c r="C46" s="89"/>
-      <c r="D46" s="89"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="196"/>
-      <c r="G46" s="196"/>
-      <c r="H46" s="196"/>
-      <c r="I46" s="195"/>
+      <c r="B46" s="151"/>
+      <c r="C46" s="151"/>
+      <c r="D46" s="151"/>
+      <c r="E46" s="152"/>
+      <c r="F46" s="107"/>
+      <c r="G46" s="107"/>
+      <c r="H46" s="107"/>
+      <c r="I46" s="88"/>
       <c r="J46" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K46" s="5"/>
     </row>
     <row r="47" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="88">
+      <c r="A47" s="150">
         <v>13</v>
       </c>
-      <c r="B47" s="89"/>
-      <c r="C47" s="89"/>
-      <c r="D47" s="89"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="196"/>
-      <c r="G47" s="196"/>
-      <c r="H47" s="196"/>
-      <c r="I47" s="195"/>
+      <c r="B47" s="151"/>
+      <c r="C47" s="151"/>
+      <c r="D47" s="151"/>
+      <c r="E47" s="152"/>
+      <c r="F47" s="107"/>
+      <c r="G47" s="107"/>
+      <c r="H47" s="107"/>
+      <c r="I47" s="88"/>
       <c r="J47" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K47" s="5"/>
     </row>
     <row r="48" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="88">
+      <c r="A48" s="150">
         <v>14</v>
       </c>
-      <c r="B48" s="89"/>
-      <c r="C48" s="89"/>
-      <c r="D48" s="89"/>
-      <c r="E48" s="90"/>
-      <c r="F48" s="196"/>
-      <c r="G48" s="196"/>
-      <c r="H48" s="196"/>
-      <c r="I48" s="195"/>
+      <c r="B48" s="151"/>
+      <c r="C48" s="151"/>
+      <c r="D48" s="151"/>
+      <c r="E48" s="152"/>
+      <c r="F48" s="107"/>
+      <c r="G48" s="107"/>
+      <c r="H48" s="107"/>
+      <c r="I48" s="88"/>
       <c r="J48" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K48" s="5"/>
     </row>
     <row r="49" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="88">
+      <c r="A49" s="150">
         <v>15</v>
       </c>
-      <c r="B49" s="89"/>
-      <c r="C49" s="89"/>
-      <c r="D49" s="89"/>
-      <c r="E49" s="90"/>
-      <c r="F49" s="192"/>
-      <c r="G49" s="193"/>
-      <c r="H49" s="194"/>
-      <c r="I49" s="195"/>
+      <c r="B49" s="151"/>
+      <c r="C49" s="151"/>
+      <c r="D49" s="151"/>
+      <c r="E49" s="152"/>
+      <c r="F49" s="102"/>
+      <c r="G49" s="103"/>
+      <c r="H49" s="104"/>
+      <c r="I49" s="88"/>
       <c r="J49" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K49" s="5"/>
     </row>
     <row r="50" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="88">
+      <c r="A50" s="150">
         <v>16</v>
       </c>
-      <c r="B50" s="89"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="89"/>
-      <c r="E50" s="90"/>
-      <c r="F50" s="192"/>
-      <c r="G50" s="193"/>
-      <c r="H50" s="194"/>
-      <c r="I50" s="195"/>
+      <c r="B50" s="151"/>
+      <c r="C50" s="151"/>
+      <c r="D50" s="151"/>
+      <c r="E50" s="152"/>
+      <c r="F50" s="102"/>
+      <c r="G50" s="103"/>
+      <c r="H50" s="104"/>
+      <c r="I50" s="88"/>
       <c r="J50" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K50" s="5"/>
     </row>
     <row r="51" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="88">
+      <c r="A51" s="150">
         <v>17</v>
       </c>
-      <c r="B51" s="89"/>
-      <c r="C51" s="89"/>
-      <c r="D51" s="89"/>
-      <c r="E51" s="90"/>
-      <c r="F51" s="192"/>
-      <c r="G51" s="193"/>
-      <c r="H51" s="194"/>
-      <c r="I51" s="195"/>
+      <c r="B51" s="151"/>
+      <c r="C51" s="151"/>
+      <c r="D51" s="151"/>
+      <c r="E51" s="152"/>
+      <c r="F51" s="102"/>
+      <c r="G51" s="103"/>
+      <c r="H51" s="104"/>
+      <c r="I51" s="88"/>
       <c r="J51" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K51" s="5"/>
     </row>
     <row r="52" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="88">
+      <c r="A52" s="150">
         <v>18</v>
       </c>
-      <c r="B52" s="89"/>
-      <c r="C52" s="89"/>
-      <c r="D52" s="89"/>
-      <c r="E52" s="90"/>
-      <c r="F52" s="192"/>
-      <c r="G52" s="193"/>
-      <c r="H52" s="194"/>
-      <c r="I52" s="195"/>
+      <c r="B52" s="151"/>
+      <c r="C52" s="151"/>
+      <c r="D52" s="151"/>
+      <c r="E52" s="152"/>
+      <c r="F52" s="102"/>
+      <c r="G52" s="103"/>
+      <c r="H52" s="104"/>
+      <c r="I52" s="88"/>
       <c r="J52" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K52" s="5"/>
     </row>
     <row r="53" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="88">
+      <c r="A53" s="150">
         <v>19</v>
       </c>
-      <c r="B53" s="89"/>
-      <c r="C53" s="89"/>
-      <c r="D53" s="89"/>
-      <c r="E53" s="90"/>
-      <c r="F53" s="192"/>
-      <c r="G53" s="193"/>
-      <c r="H53" s="194"/>
-      <c r="I53" s="195"/>
+      <c r="B53" s="151"/>
+      <c r="C53" s="151"/>
+      <c r="D53" s="151"/>
+      <c r="E53" s="152"/>
+      <c r="F53" s="102"/>
+      <c r="G53" s="103"/>
+      <c r="H53" s="104"/>
+      <c r="I53" s="88"/>
       <c r="J53" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K53" s="5"/>
     </row>
     <row r="54" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="88">
+      <c r="A54" s="150">
         <v>20</v>
       </c>
-      <c r="B54" s="89"/>
-      <c r="C54" s="89"/>
-      <c r="D54" s="89"/>
-      <c r="E54" s="90"/>
-      <c r="F54" s="192"/>
-      <c r="G54" s="193"/>
-      <c r="H54" s="194"/>
-      <c r="I54" s="195"/>
+      <c r="B54" s="151"/>
+      <c r="C54" s="151"/>
+      <c r="D54" s="151"/>
+      <c r="E54" s="152"/>
+      <c r="F54" s="102"/>
+      <c r="G54" s="103"/>
+      <c r="H54" s="104"/>
+      <c r="I54" s="88"/>
       <c r="J54" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K54" s="5"/>
     </row>
     <row r="55" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="88">
+      <c r="A55" s="150">
         <v>21</v>
       </c>
-      <c r="B55" s="89"/>
-      <c r="C55" s="89"/>
-      <c r="D55" s="89"/>
-      <c r="E55" s="90"/>
-      <c r="F55" s="192"/>
-      <c r="G55" s="193"/>
-      <c r="H55" s="194"/>
-      <c r="I55" s="195"/>
+      <c r="B55" s="151"/>
+      <c r="C55" s="151"/>
+      <c r="D55" s="151"/>
+      <c r="E55" s="152"/>
+      <c r="F55" s="102"/>
+      <c r="G55" s="103"/>
+      <c r="H55" s="104"/>
+      <c r="I55" s="88"/>
       <c r="J55" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K55" s="5"/>
     </row>
     <row r="56" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="88">
+      <c r="A56" s="150">
         <v>22</v>
       </c>
-      <c r="B56" s="89"/>
-      <c r="C56" s="89"/>
-      <c r="D56" s="89"/>
-      <c r="E56" s="90"/>
-      <c r="F56" s="192"/>
-      <c r="G56" s="193"/>
-      <c r="H56" s="194"/>
-      <c r="I56" s="195"/>
+      <c r="B56" s="151"/>
+      <c r="C56" s="151"/>
+      <c r="D56" s="151"/>
+      <c r="E56" s="152"/>
+      <c r="F56" s="102"/>
+      <c r="G56" s="103"/>
+      <c r="H56" s="104"/>
+      <c r="I56" s="88"/>
       <c r="J56" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K56" s="5"/>
     </row>
     <row r="57" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="88">
+      <c r="A57" s="150">
         <v>23</v>
       </c>
-      <c r="B57" s="89"/>
-      <c r="C57" s="89"/>
-      <c r="D57" s="89"/>
-      <c r="E57" s="90"/>
-      <c r="F57" s="192"/>
-      <c r="G57" s="193"/>
-      <c r="H57" s="194"/>
-      <c r="I57" s="195"/>
+      <c r="B57" s="151"/>
+      <c r="C57" s="151"/>
+      <c r="D57" s="151"/>
+      <c r="E57" s="152"/>
+      <c r="F57" s="102"/>
+      <c r="G57" s="103"/>
+      <c r="H57" s="104"/>
+      <c r="I57" s="88"/>
       <c r="J57" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K57" s="5"/>
     </row>
     <row r="58" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="88">
+      <c r="A58" s="150">
         <v>24</v>
       </c>
-      <c r="B58" s="89"/>
-      <c r="C58" s="89"/>
-      <c r="D58" s="89"/>
-      <c r="E58" s="90"/>
-      <c r="F58" s="192"/>
-      <c r="G58" s="193"/>
-      <c r="H58" s="194"/>
-      <c r="I58" s="195"/>
+      <c r="B58" s="151"/>
+      <c r="C58" s="151"/>
+      <c r="D58" s="151"/>
+      <c r="E58" s="152"/>
+      <c r="F58" s="102"/>
+      <c r="G58" s="103"/>
+      <c r="H58" s="104"/>
+      <c r="I58" s="88"/>
       <c r="J58" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K58" s="5"/>
     </row>
     <row r="59" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="88">
+      <c r="A59" s="150">
         <v>25</v>
       </c>
-      <c r="B59" s="89"/>
-      <c r="C59" s="89"/>
-      <c r="D59" s="89"/>
-      <c r="E59" s="90"/>
-      <c r="F59" s="192"/>
-      <c r="G59" s="193"/>
-      <c r="H59" s="194"/>
-      <c r="I59" s="195"/>
+      <c r="B59" s="151"/>
+      <c r="C59" s="151"/>
+      <c r="D59" s="151"/>
+      <c r="E59" s="152"/>
+      <c r="F59" s="102"/>
+      <c r="G59" s="103"/>
+      <c r="H59" s="104"/>
+      <c r="I59" s="88"/>
       <c r="J59" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K59" s="5"/>
     </row>
     <row r="60" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="88">
+      <c r="A60" s="150">
         <v>26</v>
       </c>
-      <c r="B60" s="89"/>
-      <c r="C60" s="89"/>
-      <c r="D60" s="89"/>
-      <c r="E60" s="90"/>
-      <c r="F60" s="192"/>
-      <c r="G60" s="193"/>
-      <c r="H60" s="194"/>
-      <c r="I60" s="195"/>
+      <c r="B60" s="151"/>
+      <c r="C60" s="151"/>
+      <c r="D60" s="151"/>
+      <c r="E60" s="152"/>
+      <c r="F60" s="102"/>
+      <c r="G60" s="103"/>
+      <c r="H60" s="104"/>
+      <c r="I60" s="88"/>
       <c r="J60" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K60" s="5"/>
     </row>
     <row r="61" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="88">
+      <c r="A61" s="150">
         <v>27</v>
       </c>
-      <c r="B61" s="89"/>
-      <c r="C61" s="89"/>
-      <c r="D61" s="89"/>
-      <c r="E61" s="90"/>
-      <c r="F61" s="192"/>
-      <c r="G61" s="193"/>
-      <c r="H61" s="194"/>
-      <c r="I61" s="195"/>
+      <c r="B61" s="151"/>
+      <c r="C61" s="151"/>
+      <c r="D61" s="151"/>
+      <c r="E61" s="152"/>
+      <c r="F61" s="102"/>
+      <c r="G61" s="103"/>
+      <c r="H61" s="104"/>
+      <c r="I61" s="88"/>
       <c r="J61" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K61" s="5"/>
     </row>
     <row r="62" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="88">
+      <c r="A62" s="150">
         <v>28</v>
       </c>
-      <c r="B62" s="89"/>
-      <c r="C62" s="89"/>
-      <c r="D62" s="89"/>
-      <c r="E62" s="90"/>
-      <c r="F62" s="192"/>
-      <c r="G62" s="193"/>
-      <c r="H62" s="194"/>
-      <c r="I62" s="195"/>
+      <c r="B62" s="151"/>
+      <c r="C62" s="151"/>
+      <c r="D62" s="151"/>
+      <c r="E62" s="152"/>
+      <c r="F62" s="102"/>
+      <c r="G62" s="103"/>
+      <c r="H62" s="104"/>
+      <c r="I62" s="88"/>
       <c r="J62" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K62" s="5"/>
     </row>
     <row r="63" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="88">
+      <c r="A63" s="150">
         <v>29</v>
       </c>
-      <c r="B63" s="89"/>
-      <c r="C63" s="89"/>
-      <c r="D63" s="89"/>
-      <c r="E63" s="90"/>
-      <c r="F63" s="192"/>
-      <c r="G63" s="193"/>
-      <c r="H63" s="194"/>
-      <c r="I63" s="195"/>
+      <c r="B63" s="151"/>
+      <c r="C63" s="151"/>
+      <c r="D63" s="151"/>
+      <c r="E63" s="152"/>
+      <c r="F63" s="102"/>
+      <c r="G63" s="103"/>
+      <c r="H63" s="104"/>
+      <c r="I63" s="88"/>
       <c r="J63" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K63" s="5"/>
     </row>
     <row r="64" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="88">
+      <c r="A64" s="150">
         <v>30</v>
       </c>
-      <c r="B64" s="89"/>
-      <c r="C64" s="89"/>
-      <c r="D64" s="89"/>
-      <c r="E64" s="90"/>
-      <c r="F64" s="192"/>
-      <c r="G64" s="193"/>
-      <c r="H64" s="194"/>
-      <c r="I64" s="195"/>
+      <c r="B64" s="151"/>
+      <c r="C64" s="151"/>
+      <c r="D64" s="151"/>
+      <c r="E64" s="152"/>
+      <c r="F64" s="102"/>
+      <c r="G64" s="103"/>
+      <c r="H64" s="104"/>
+      <c r="I64" s="88"/>
       <c r="J64" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K64" s="5"/>
     </row>
     <row r="65" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="88">
+      <c r="A65" s="150">
         <v>31</v>
       </c>
-      <c r="B65" s="89"/>
-      <c r="C65" s="89"/>
-      <c r="D65" s="89"/>
-      <c r="E65" s="90"/>
-      <c r="F65" s="192"/>
-      <c r="G65" s="193"/>
-      <c r="H65" s="194"/>
-      <c r="I65" s="195"/>
+      <c r="B65" s="151"/>
+      <c r="C65" s="151"/>
+      <c r="D65" s="151"/>
+      <c r="E65" s="152"/>
+      <c r="F65" s="102"/>
+      <c r="G65" s="103"/>
+      <c r="H65" s="104"/>
+      <c r="I65" s="88"/>
       <c r="J65" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K65" s="5"/>
     </row>
     <row r="66" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="88">
+      <c r="A66" s="150">
         <v>32</v>
       </c>
-      <c r="B66" s="89"/>
-      <c r="C66" s="89"/>
-      <c r="D66" s="89"/>
-      <c r="E66" s="90"/>
-      <c r="F66" s="192"/>
-      <c r="G66" s="193"/>
-      <c r="H66" s="194"/>
-      <c r="I66" s="195"/>
+      <c r="B66" s="151"/>
+      <c r="C66" s="151"/>
+      <c r="D66" s="151"/>
+      <c r="E66" s="152"/>
+      <c r="F66" s="102"/>
+      <c r="G66" s="103"/>
+      <c r="H66" s="104"/>
+      <c r="I66" s="88"/>
       <c r="J66" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K66" s="5"/>
     </row>
     <row r="67" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="88">
+      <c r="A67" s="150">
         <v>33</v>
       </c>
-      <c r="B67" s="89"/>
-      <c r="C67" s="89"/>
-      <c r="D67" s="89"/>
-      <c r="E67" s="90"/>
-      <c r="F67" s="192"/>
-      <c r="G67" s="193"/>
-      <c r="H67" s="194"/>
-      <c r="I67" s="195"/>
+      <c r="B67" s="151"/>
+      <c r="C67" s="151"/>
+      <c r="D67" s="151"/>
+      <c r="E67" s="152"/>
+      <c r="F67" s="102"/>
+      <c r="G67" s="103"/>
+      <c r="H67" s="104"/>
+      <c r="I67" s="88"/>
       <c r="J67" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K67" s="5"/>
     </row>
     <row r="68" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="88">
+      <c r="A68" s="150">
         <v>34</v>
       </c>
-      <c r="B68" s="89"/>
-      <c r="C68" s="89"/>
-      <c r="D68" s="89"/>
-      <c r="E68" s="90"/>
-      <c r="F68" s="192"/>
-      <c r="G68" s="193"/>
-      <c r="H68" s="194"/>
-      <c r="I68" s="195"/>
+      <c r="B68" s="151"/>
+      <c r="C68" s="151"/>
+      <c r="D68" s="151"/>
+      <c r="E68" s="152"/>
+      <c r="F68" s="102"/>
+      <c r="G68" s="103"/>
+      <c r="H68" s="104"/>
+      <c r="I68" s="88"/>
       <c r="J68" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K68" s="5"/>
     </row>
     <row r="69" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="88">
+      <c r="A69" s="150">
         <v>35</v>
       </c>
-      <c r="B69" s="89"/>
-      <c r="C69" s="89"/>
-      <c r="D69" s="89"/>
-      <c r="E69" s="90"/>
-      <c r="F69" s="192"/>
-      <c r="G69" s="193"/>
-      <c r="H69" s="194"/>
-      <c r="I69" s="195"/>
+      <c r="B69" s="151"/>
+      <c r="C69" s="151"/>
+      <c r="D69" s="151"/>
+      <c r="E69" s="152"/>
+      <c r="F69" s="102"/>
+      <c r="G69" s="103"/>
+      <c r="H69" s="104"/>
+      <c r="I69" s="88"/>
       <c r="J69" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K69" s="5"/>
     </row>
     <row r="70" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="88">
+      <c r="A70" s="150">
         <v>36</v>
       </c>
-      <c r="B70" s="89"/>
-      <c r="C70" s="89"/>
-      <c r="D70" s="89"/>
-      <c r="E70" s="90"/>
-      <c r="F70" s="192"/>
-      <c r="G70" s="193"/>
-      <c r="H70" s="194"/>
-      <c r="I70" s="195"/>
+      <c r="B70" s="151"/>
+      <c r="C70" s="151"/>
+      <c r="D70" s="151"/>
+      <c r="E70" s="152"/>
+      <c r="F70" s="102"/>
+      <c r="G70" s="103"/>
+      <c r="H70" s="104"/>
+      <c r="I70" s="88"/>
       <c r="J70" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K70" s="5"/>
     </row>
     <row r="71" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="88">
+      <c r="A71" s="150">
         <v>37</v>
       </c>
-      <c r="B71" s="89"/>
-      <c r="C71" s="89"/>
-      <c r="D71" s="89"/>
-      <c r="E71" s="90"/>
-      <c r="F71" s="192"/>
-      <c r="G71" s="193"/>
-      <c r="H71" s="194"/>
-      <c r="I71" s="195"/>
+      <c r="B71" s="151"/>
+      <c r="C71" s="151"/>
+      <c r="D71" s="151"/>
+      <c r="E71" s="152"/>
+      <c r="F71" s="102"/>
+      <c r="G71" s="103"/>
+      <c r="H71" s="104"/>
+      <c r="I71" s="88"/>
       <c r="J71" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K71" s="5"/>
     </row>
     <row r="72" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="88">
+      <c r="A72" s="150">
         <v>38</v>
       </c>
-      <c r="B72" s="89"/>
-      <c r="C72" s="89"/>
-      <c r="D72" s="89"/>
-      <c r="E72" s="90"/>
-      <c r="F72" s="192"/>
-      <c r="G72" s="193"/>
-      <c r="H72" s="194"/>
-      <c r="I72" s="195"/>
+      <c r="B72" s="151"/>
+      <c r="C72" s="151"/>
+      <c r="D72" s="151"/>
+      <c r="E72" s="152"/>
+      <c r="F72" s="102"/>
+      <c r="G72" s="103"/>
+      <c r="H72" s="104"/>
+      <c r="I72" s="88"/>
       <c r="J72" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K72" s="5"/>
     </row>
     <row r="73" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="88">
+      <c r="A73" s="150">
         <v>39</v>
       </c>
-      <c r="B73" s="89"/>
-      <c r="C73" s="89"/>
-      <c r="D73" s="89"/>
-      <c r="E73" s="90"/>
-      <c r="F73" s="192"/>
-      <c r="G73" s="193"/>
-      <c r="H73" s="194"/>
-      <c r="I73" s="195"/>
+      <c r="B73" s="151"/>
+      <c r="C73" s="151"/>
+      <c r="D73" s="151"/>
+      <c r="E73" s="152"/>
+      <c r="F73" s="102"/>
+      <c r="G73" s="103"/>
+      <c r="H73" s="104"/>
+      <c r="I73" s="88"/>
       <c r="J73" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K73" s="5"/>
     </row>
     <row r="74" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="88">
+      <c r="A74" s="150">
         <v>40</v>
       </c>
-      <c r="B74" s="89"/>
-      <c r="C74" s="89"/>
-      <c r="D74" s="89"/>
-      <c r="E74" s="90"/>
-      <c r="F74" s="192"/>
-      <c r="G74" s="193"/>
-      <c r="H74" s="194"/>
-      <c r="I74" s="195"/>
+      <c r="B74" s="151"/>
+      <c r="C74" s="151"/>
+      <c r="D74" s="151"/>
+      <c r="E74" s="152"/>
+      <c r="F74" s="102"/>
+      <c r="G74" s="103"/>
+      <c r="H74" s="104"/>
+      <c r="I74" s="88"/>
       <c r="J74" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K74" s="5"/>
     </row>
     <row r="75" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="88">
+      <c r="A75" s="150">
         <v>41</v>
       </c>
-      <c r="B75" s="89"/>
-      <c r="C75" s="89"/>
-      <c r="D75" s="89"/>
-      <c r="E75" s="90"/>
-      <c r="F75" s="192"/>
-      <c r="G75" s="193"/>
-      <c r="H75" s="194"/>
-      <c r="I75" s="195"/>
+      <c r="B75" s="151"/>
+      <c r="C75" s="151"/>
+      <c r="D75" s="151"/>
+      <c r="E75" s="152"/>
+      <c r="F75" s="102"/>
+      <c r="G75" s="103"/>
+      <c r="H75" s="104"/>
+      <c r="I75" s="88"/>
       <c r="J75" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K75" s="5"/>
     </row>
     <row r="76" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="88">
+      <c r="A76" s="150">
         <v>42</v>
       </c>
-      <c r="B76" s="89"/>
-      <c r="C76" s="89"/>
-      <c r="D76" s="89"/>
-      <c r="E76" s="90"/>
-      <c r="F76" s="192"/>
-      <c r="G76" s="193"/>
-      <c r="H76" s="194"/>
-      <c r="I76" s="195"/>
+      <c r="B76" s="151"/>
+      <c r="C76" s="151"/>
+      <c r="D76" s="151"/>
+      <c r="E76" s="152"/>
+      <c r="F76" s="102"/>
+      <c r="G76" s="103"/>
+      <c r="H76" s="104"/>
+      <c r="I76" s="88"/>
       <c r="J76" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K76" s="5"/>
     </row>
     <row r="77" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="88">
+      <c r="A77" s="150">
         <v>43</v>
       </c>
-      <c r="B77" s="89"/>
-      <c r="C77" s="89"/>
-      <c r="D77" s="89"/>
-      <c r="E77" s="90"/>
-      <c r="F77" s="192"/>
-      <c r="G77" s="193"/>
-      <c r="H77" s="194"/>
-      <c r="I77" s="195"/>
+      <c r="B77" s="151"/>
+      <c r="C77" s="151"/>
+      <c r="D77" s="151"/>
+      <c r="E77" s="152"/>
+      <c r="F77" s="102"/>
+      <c r="G77" s="103"/>
+      <c r="H77" s="104"/>
+      <c r="I77" s="88"/>
       <c r="J77" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K77" s="5"/>
     </row>
     <row r="78" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="88">
+      <c r="A78" s="150">
         <v>44</v>
       </c>
-      <c r="B78" s="89"/>
-      <c r="C78" s="89"/>
-      <c r="D78" s="89"/>
-      <c r="E78" s="90"/>
-      <c r="F78" s="192"/>
-      <c r="G78" s="193"/>
-      <c r="H78" s="194"/>
-      <c r="I78" s="195"/>
+      <c r="B78" s="151"/>
+      <c r="C78" s="151"/>
+      <c r="D78" s="151"/>
+      <c r="E78" s="152"/>
+      <c r="F78" s="102"/>
+      <c r="G78" s="103"/>
+      <c r="H78" s="104"/>
+      <c r="I78" s="88"/>
       <c r="J78" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K78" s="5"/>
     </row>
     <row r="79" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="88">
+      <c r="A79" s="150">
         <v>45</v>
       </c>
-      <c r="B79" s="89"/>
-      <c r="C79" s="89"/>
-      <c r="D79" s="89"/>
-      <c r="E79" s="90"/>
-      <c r="F79" s="192"/>
-      <c r="G79" s="193"/>
-      <c r="H79" s="194"/>
-      <c r="I79" s="195"/>
+      <c r="B79" s="151"/>
+      <c r="C79" s="151"/>
+      <c r="D79" s="151"/>
+      <c r="E79" s="152"/>
+      <c r="F79" s="102"/>
+      <c r="G79" s="103"/>
+      <c r="H79" s="104"/>
+      <c r="I79" s="88"/>
       <c r="J79" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K79" s="5"/>
     </row>
     <row r="80" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="88">
+      <c r="A80" s="150">
         <v>46</v>
       </c>
-      <c r="B80" s="89"/>
-      <c r="C80" s="89"/>
-      <c r="D80" s="89"/>
-      <c r="E80" s="90"/>
-      <c r="F80" s="192"/>
-      <c r="G80" s="193"/>
-      <c r="H80" s="194"/>
-      <c r="I80" s="195"/>
+      <c r="B80" s="151"/>
+      <c r="C80" s="151"/>
+      <c r="D80" s="151"/>
+      <c r="E80" s="152"/>
+      <c r="F80" s="102"/>
+      <c r="G80" s="103"/>
+      <c r="H80" s="104"/>
+      <c r="I80" s="88"/>
       <c r="J80" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K80" s="5"/>
     </row>
     <row r="81" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="88">
+      <c r="A81" s="150">
         <v>47</v>
       </c>
-      <c r="B81" s="89"/>
-      <c r="C81" s="89"/>
-      <c r="D81" s="89"/>
-      <c r="E81" s="90"/>
-      <c r="F81" s="192"/>
-      <c r="G81" s="193"/>
-      <c r="H81" s="194"/>
-      <c r="I81" s="195"/>
+      <c r="B81" s="151"/>
+      <c r="C81" s="151"/>
+      <c r="D81" s="151"/>
+      <c r="E81" s="152"/>
+      <c r="F81" s="102"/>
+      <c r="G81" s="103"/>
+      <c r="H81" s="104"/>
+      <c r="I81" s="88"/>
       <c r="J81" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K81" s="5"/>
     </row>
     <row r="82" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="88">
+      <c r="A82" s="150">
         <v>48</v>
       </c>
-      <c r="B82" s="89"/>
-      <c r="C82" s="89"/>
-      <c r="D82" s="89"/>
-      <c r="E82" s="90"/>
-      <c r="F82" s="192"/>
-      <c r="G82" s="193"/>
-      <c r="H82" s="194"/>
-      <c r="I82" s="195"/>
+      <c r="B82" s="151"/>
+      <c r="C82" s="151"/>
+      <c r="D82" s="151"/>
+      <c r="E82" s="152"/>
+      <c r="F82" s="102"/>
+      <c r="G82" s="103"/>
+      <c r="H82" s="104"/>
+      <c r="I82" s="88"/>
       <c r="J82" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K82" s="5"/>
     </row>
     <row r="83" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="88">
+      <c r="A83" s="150">
         <v>49</v>
       </c>
-      <c r="B83" s="89"/>
-      <c r="C83" s="89"/>
-      <c r="D83" s="89"/>
-      <c r="E83" s="90"/>
-      <c r="F83" s="192"/>
-      <c r="G83" s="193"/>
-      <c r="H83" s="194"/>
-      <c r="I83" s="195"/>
+      <c r="B83" s="151"/>
+      <c r="C83" s="151"/>
+      <c r="D83" s="151"/>
+      <c r="E83" s="152"/>
+      <c r="F83" s="102"/>
+      <c r="G83" s="103"/>
+      <c r="H83" s="104"/>
+      <c r="I83" s="88"/>
       <c r="J83" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K83" s="5"/>
     </row>
     <row r="84" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="88">
+      <c r="A84" s="150">
         <v>50</v>
       </c>
-      <c r="B84" s="89"/>
-      <c r="C84" s="89"/>
-      <c r="D84" s="89"/>
-      <c r="E84" s="90"/>
-      <c r="F84" s="192"/>
-      <c r="G84" s="193"/>
-      <c r="H84" s="194"/>
-      <c r="I84" s="195"/>
+      <c r="B84" s="151"/>
+      <c r="C84" s="151"/>
+      <c r="D84" s="151"/>
+      <c r="E84" s="152"/>
+      <c r="F84" s="102"/>
+      <c r="G84" s="103"/>
+      <c r="H84" s="104"/>
+      <c r="I84" s="88"/>
       <c r="J84" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K84" s="5"/>
     </row>
     <row r="85" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="88">
+      <c r="A85" s="150">
         <v>51</v>
       </c>
-      <c r="B85" s="89"/>
-      <c r="C85" s="89"/>
-      <c r="D85" s="89"/>
-      <c r="E85" s="90"/>
-      <c r="F85" s="192"/>
-      <c r="G85" s="193"/>
-      <c r="H85" s="194"/>
-      <c r="I85" s="195"/>
+      <c r="B85" s="151"/>
+      <c r="C85" s="151"/>
+      <c r="D85" s="151"/>
+      <c r="E85" s="152"/>
+      <c r="F85" s="102"/>
+      <c r="G85" s="103"/>
+      <c r="H85" s="104"/>
+      <c r="I85" s="88"/>
       <c r="J85" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K85" s="5"/>
     </row>
     <row r="86" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="88">
+      <c r="A86" s="150">
         <v>52</v>
       </c>
-      <c r="B86" s="89"/>
-      <c r="C86" s="89"/>
-      <c r="D86" s="89"/>
-      <c r="E86" s="90"/>
-      <c r="F86" s="192"/>
-      <c r="G86" s="193"/>
-      <c r="H86" s="194"/>
-      <c r="I86" s="195"/>
+      <c r="B86" s="151"/>
+      <c r="C86" s="151"/>
+      <c r="D86" s="151"/>
+      <c r="E86" s="152"/>
+      <c r="F86" s="102"/>
+      <c r="G86" s="103"/>
+      <c r="H86" s="104"/>
+      <c r="I86" s="88"/>
       <c r="J86" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K86" s="5"/>
     </row>
     <row r="87" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="88">
+      <c r="A87" s="150">
         <v>53</v>
       </c>
-      <c r="B87" s="89"/>
-      <c r="C87" s="89"/>
-      <c r="D87" s="89"/>
-      <c r="E87" s="90"/>
-      <c r="F87" s="192"/>
-      <c r="G87" s="193"/>
-      <c r="H87" s="194"/>
-      <c r="I87" s="195"/>
+      <c r="B87" s="151"/>
+      <c r="C87" s="151"/>
+      <c r="D87" s="151"/>
+      <c r="E87" s="152"/>
+      <c r="F87" s="102"/>
+      <c r="G87" s="103"/>
+      <c r="H87" s="104"/>
+      <c r="I87" s="88"/>
       <c r="J87" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K87" s="5"/>
     </row>
     <row r="88" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="88">
+      <c r="A88" s="150">
         <v>54</v>
       </c>
-      <c r="B88" s="89"/>
-      <c r="C88" s="89"/>
-      <c r="D88" s="89"/>
-      <c r="E88" s="90"/>
-      <c r="F88" s="192"/>
-      <c r="G88" s="193"/>
-      <c r="H88" s="194"/>
-      <c r="I88" s="195"/>
+      <c r="B88" s="151"/>
+      <c r="C88" s="151"/>
+      <c r="D88" s="151"/>
+      <c r="E88" s="152"/>
+      <c r="F88" s="102"/>
+      <c r="G88" s="103"/>
+      <c r="H88" s="104"/>
+      <c r="I88" s="88"/>
       <c r="J88" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K88" s="5"/>
     </row>
     <row r="89" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="88">
+      <c r="A89" s="150">
         <v>55</v>
       </c>
-      <c r="B89" s="89"/>
-      <c r="C89" s="89"/>
-      <c r="D89" s="89"/>
-      <c r="E89" s="90"/>
-      <c r="F89" s="192"/>
-      <c r="G89" s="193"/>
-      <c r="H89" s="194"/>
-      <c r="I89" s="195"/>
+      <c r="B89" s="151"/>
+      <c r="C89" s="151"/>
+      <c r="D89" s="151"/>
+      <c r="E89" s="152"/>
+      <c r="F89" s="102"/>
+      <c r="G89" s="103"/>
+      <c r="H89" s="104"/>
+      <c r="I89" s="88"/>
       <c r="J89" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K89" s="5"/>
     </row>
     <row r="90" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="88">
+      <c r="A90" s="150">
         <v>56</v>
       </c>
-      <c r="B90" s="89"/>
-      <c r="C90" s="89"/>
-      <c r="D90" s="89"/>
-      <c r="E90" s="90"/>
-      <c r="F90" s="192"/>
-      <c r="G90" s="193"/>
-      <c r="H90" s="194"/>
-      <c r="I90" s="195"/>
+      <c r="B90" s="151"/>
+      <c r="C90" s="151"/>
+      <c r="D90" s="151"/>
+      <c r="E90" s="152"/>
+      <c r="F90" s="102"/>
+      <c r="G90" s="103"/>
+      <c r="H90" s="104"/>
+      <c r="I90" s="88"/>
       <c r="J90" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K90" s="5"/>
     </row>
     <row r="91" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="88">
+      <c r="A91" s="150">
         <v>57</v>
       </c>
-      <c r="B91" s="89"/>
-      <c r="C91" s="89"/>
-      <c r="D91" s="89"/>
-      <c r="E91" s="90"/>
-      <c r="F91" s="192"/>
-      <c r="G91" s="193"/>
-      <c r="H91" s="194"/>
-      <c r="I91" s="195"/>
+      <c r="B91" s="151"/>
+      <c r="C91" s="151"/>
+      <c r="D91" s="151"/>
+      <c r="E91" s="152"/>
+      <c r="F91" s="102"/>
+      <c r="G91" s="103"/>
+      <c r="H91" s="104"/>
+      <c r="I91" s="88"/>
       <c r="J91" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K91" s="5"/>
     </row>
     <row r="92" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="88">
+      <c r="A92" s="150">
         <v>58</v>
       </c>
-      <c r="B92" s="89"/>
-      <c r="C92" s="89"/>
-      <c r="D92" s="89"/>
-      <c r="E92" s="90"/>
-      <c r="F92" s="192"/>
-      <c r="G92" s="193"/>
-      <c r="H92" s="194"/>
-      <c r="I92" s="195"/>
+      <c r="B92" s="151"/>
+      <c r="C92" s="151"/>
+      <c r="D92" s="151"/>
+      <c r="E92" s="152"/>
+      <c r="F92" s="102"/>
+      <c r="G92" s="103"/>
+      <c r="H92" s="104"/>
+      <c r="I92" s="88"/>
       <c r="J92" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K92" s="5"/>
     </row>
     <row r="93" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="88">
+      <c r="A93" s="150">
         <v>59</v>
       </c>
-      <c r="B93" s="89"/>
-      <c r="C93" s="89"/>
-      <c r="D93" s="89"/>
-      <c r="E93" s="90"/>
-      <c r="F93" s="192"/>
-      <c r="G93" s="193"/>
-      <c r="H93" s="194"/>
-      <c r="I93" s="195"/>
+      <c r="B93" s="151"/>
+      <c r="C93" s="151"/>
+      <c r="D93" s="151"/>
+      <c r="E93" s="152"/>
+      <c r="F93" s="102"/>
+      <c r="G93" s="103"/>
+      <c r="H93" s="104"/>
+      <c r="I93" s="88"/>
       <c r="J93" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K93" s="5"/>
     </row>
     <row r="94" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="88">
+      <c r="A94" s="150">
         <v>60</v>
       </c>
-      <c r="B94" s="89"/>
-      <c r="C94" s="89"/>
-      <c r="D94" s="89"/>
-      <c r="E94" s="90"/>
-      <c r="F94" s="192"/>
-      <c r="G94" s="193"/>
-      <c r="H94" s="194"/>
-      <c r="I94" s="195"/>
+      <c r="B94" s="151"/>
+      <c r="C94" s="151"/>
+      <c r="D94" s="151"/>
+      <c r="E94" s="152"/>
+      <c r="F94" s="102"/>
+      <c r="G94" s="103"/>
+      <c r="H94" s="104"/>
+      <c r="I94" s="88"/>
       <c r="J94" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K94" s="5"/>
     </row>
     <row r="95" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="88">
+      <c r="A95" s="150">
         <v>61</v>
       </c>
-      <c r="B95" s="89"/>
-      <c r="C95" s="89"/>
-      <c r="D95" s="89"/>
-      <c r="E95" s="90"/>
-      <c r="F95" s="192"/>
-      <c r="G95" s="193"/>
-      <c r="H95" s="194"/>
-      <c r="I95" s="195"/>
+      <c r="B95" s="151"/>
+      <c r="C95" s="151"/>
+      <c r="D95" s="151"/>
+      <c r="E95" s="152"/>
+      <c r="F95" s="102"/>
+      <c r="G95" s="103"/>
+      <c r="H95" s="104"/>
+      <c r="I95" s="88"/>
       <c r="J95" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K95" s="5"/>
     </row>
     <row r="96" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="88">
+      <c r="A96" s="150">
         <v>62</v>
       </c>
-      <c r="B96" s="89"/>
-      <c r="C96" s="89"/>
-      <c r="D96" s="89"/>
-      <c r="E96" s="90"/>
-      <c r="F96" s="192"/>
-      <c r="G96" s="193"/>
-      <c r="H96" s="194"/>
-      <c r="I96" s="195"/>
+      <c r="B96" s="151"/>
+      <c r="C96" s="151"/>
+      <c r="D96" s="151"/>
+      <c r="E96" s="152"/>
+      <c r="F96" s="102"/>
+      <c r="G96" s="103"/>
+      <c r="H96" s="104"/>
+      <c r="I96" s="88"/>
       <c r="J96" s="8" t="s">
         <v>118</v>
       </c>
@@ -23733,60 +23730,60 @@
     </row>
     <row r="97" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="25"/>
-      <c r="B97" s="158"/>
-      <c r="C97" s="158"/>
-      <c r="D97" s="158"/>
-      <c r="E97" s="158"/>
-      <c r="F97" s="158"/>
-      <c r="G97" s="158"/>
-      <c r="H97" s="158"/>
+      <c r="B97" s="105"/>
+      <c r="C97" s="105"/>
+      <c r="D97" s="105"/>
+      <c r="E97" s="105"/>
+      <c r="F97" s="105"/>
+      <c r="G97" s="105"/>
+      <c r="H97" s="105"/>
       <c r="I97" s="87"/>
       <c r="J97" s="7"/>
       <c r="K97" s="25"/>
     </row>
     <row r="98" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="159" t="s">
+      <c r="A98" s="106" t="s">
         <v>120</v>
       </c>
-      <c r="B98" s="159"/>
-      <c r="C98" s="159"/>
-      <c r="D98" s="159"/>
-      <c r="E98" s="159"/>
-      <c r="F98" s="159"/>
-      <c r="G98" s="159"/>
-      <c r="H98" s="159"/>
-      <c r="I98" s="159"/>
-      <c r="J98" s="159"/>
-      <c r="K98" s="159"/>
+      <c r="B98" s="106"/>
+      <c r="C98" s="106"/>
+      <c r="D98" s="106"/>
+      <c r="E98" s="106"/>
+      <c r="F98" s="106"/>
+      <c r="G98" s="106"/>
+      <c r="H98" s="106"/>
+      <c r="I98" s="106"/>
+      <c r="J98" s="106"/>
+      <c r="K98" s="106"/>
     </row>
     <row r="99" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A100" s="146" t="s">
+      <c r="A100" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="B100" s="147"/>
-      <c r="C100" s="147"/>
-      <c r="D100" s="147"/>
-      <c r="E100" s="147"/>
-      <c r="F100" s="147"/>
-      <c r="G100" s="147"/>
-      <c r="H100" s="147"/>
-      <c r="I100" s="147"/>
-      <c r="J100" s="147"/>
-      <c r="K100" s="148"/>
+      <c r="B100" s="90"/>
+      <c r="C100" s="90"/>
+      <c r="D100" s="90"/>
+      <c r="E100" s="90"/>
+      <c r="F100" s="90"/>
+      <c r="G100" s="90"/>
+      <c r="H100" s="90"/>
+      <c r="I100" s="90"/>
+      <c r="J100" s="90"/>
+      <c r="K100" s="91"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A101" s="149"/>
-      <c r="B101" s="150"/>
-      <c r="C101" s="150"/>
-      <c r="D101" s="150"/>
-      <c r="E101" s="150"/>
-      <c r="F101" s="150"/>
-      <c r="G101" s="150"/>
-      <c r="H101" s="150"/>
-      <c r="I101" s="150"/>
-      <c r="J101" s="150"/>
-      <c r="K101" s="151"/>
+      <c r="A101" s="92"/>
+      <c r="B101" s="93"/>
+      <c r="C101" s="93"/>
+      <c r="D101" s="93"/>
+      <c r="E101" s="93"/>
+      <c r="F101" s="93"/>
+      <c r="G101" s="93"/>
+      <c r="H101" s="93"/>
+      <c r="I101" s="93"/>
+      <c r="J101" s="93"/>
+      <c r="K101" s="94"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="84" t="s">
@@ -23807,54 +23804,106 @@
     </row>
   </sheetData>
   <mergeCells count="172">
-    <mergeCell ref="A100:K101"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="B97:E97"/>
-    <mergeCell ref="A98:K98"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A6:K7"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="A25:K26"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A93:E93"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="A94:E94"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="A95:E95"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="A90:E90"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="A92:E92"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="A87:E87"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="A88:E88"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="A89:E89"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="A85:E85"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="A86:E86"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="A84:E84"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="A79:E79"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="A81:E81"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="A76:E76"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="A73:E73"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="A74:E74"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="A75:E75"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="A70:E70"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="A71:E71"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A96:E96"/>
+    <mergeCell ref="A69:E69"/>
+    <mergeCell ref="A72:E72"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A60:E60"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A66:E66"/>
     <mergeCell ref="A39:E39"/>
     <mergeCell ref="A40:E40"/>
     <mergeCell ref="A41:E41"/>
@@ -23879,106 +23928,54 @@
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A66:E66"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="A54:E54"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="A56:E56"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A96:E96"/>
-    <mergeCell ref="A69:E69"/>
-    <mergeCell ref="A72:E72"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="A64:E64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="A70:E70"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="A71:E71"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="A67:E67"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="A76:E76"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="A77:E77"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="A73:E73"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="A74:E74"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="A75:E75"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="A79:E79"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="A81:E81"/>
-    <mergeCell ref="A87:E87"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="A88:E88"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="A85:E85"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="A86:E86"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="A84:E84"/>
-    <mergeCell ref="A93:E93"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="A94:E94"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="A95:E95"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="A90:E90"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="A91:E91"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="A92:E92"/>
-    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A6:K7"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="A100:K101"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="B97:E97"/>
+    <mergeCell ref="A98:K98"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="A25:K26"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -29584,72 +29581,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="109" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="129"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="111"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="130"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131"/>
-      <c r="K2" s="131"/>
-      <c r="L2" s="132"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="114"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="135" t="s">
+      <c r="B3" s="117" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="136"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="135" t="s">
+      <c r="C3" s="118"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="117" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="137"/>
-      <c r="J3" s="136"/>
-      <c r="K3" s="141">
+      <c r="I3" s="119"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="123">
         <v>4236654</v>
       </c>
-      <c r="L3" s="179"/>
+      <c r="L3" s="180"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="62"/>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="180"/>
-      <c r="E4" s="180"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="181"/>
-      <c r="H4" s="141" t="s">
+      <c r="C4" s="118"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="176"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="177"/>
+      <c r="H4" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="142"/>
+      <c r="I4" s="124"/>
       <c r="J4" s="23"/>
       <c r="K4" s="22" t="s">
         <v>105</v>
@@ -29658,32 +29655,32 @@
     </row>
     <row r="5" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
-      <c r="L6" s="112"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="125"/>
+      <c r="J6" s="125"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="125"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="125"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="125"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="68" t="s">
@@ -29695,14 +29692,14 @@
       <c r="F8" s="68"/>
       <c r="G8" s="68"/>
       <c r="H8" s="68"/>
-      <c r="I8" s="92" t="s">
+      <c r="I8" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92" t="s">
+      <c r="J8" s="96"/>
+      <c r="K8" s="96" t="s">
         <v>123</v>
       </c>
-      <c r="L8" s="92"/>
+      <c r="L8" s="96"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="68"/>
@@ -29726,11 +29723,11 @@
       <c r="C10" s="68"/>
       <c r="D10" s="68"/>
       <c r="E10" s="68"/>
-      <c r="F10" s="96" t="s">
+      <c r="F10" s="130" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="97"/>
-      <c r="H10" s="98"/>
+      <c r="G10" s="157"/>
+      <c r="H10" s="131"/>
       <c r="I10" s="46"/>
       <c r="J10" s="36"/>
       <c r="K10" s="4" t="s">
@@ -29743,11 +29740,11 @@
       <c r="C11" s="68"/>
       <c r="D11" s="68"/>
       <c r="E11" s="68"/>
-      <c r="F11" s="96" t="s">
+      <c r="F11" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="97"/>
-      <c r="H11" s="98"/>
+      <c r="G11" s="157"/>
+      <c r="H11" s="131"/>
       <c r="I11" s="46"/>
       <c r="J11" s="36"/>
       <c r="K11" s="4" t="s">
@@ -29760,11 +29757,11 @@
       <c r="C12" s="68"/>
       <c r="D12" s="68"/>
       <c r="E12" s="68"/>
-      <c r="F12" s="96" t="s">
+      <c r="F12" s="130" t="s">
         <v>106</v>
       </c>
-      <c r="G12" s="97"/>
-      <c r="H12" s="98"/>
+      <c r="G12" s="157"/>
+      <c r="H12" s="131"/>
       <c r="I12" s="24" t="s">
         <v>108</v>
       </c>
@@ -29783,11 +29780,11 @@
       <c r="C13" s="68"/>
       <c r="D13" s="68"/>
       <c r="E13" s="68"/>
-      <c r="F13" s="96" t="s">
+      <c r="F13" s="130" t="s">
         <v>107</v>
       </c>
-      <c r="G13" s="97"/>
-      <c r="H13" s="98"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="131"/>
       <c r="I13" s="24" t="s">
         <v>108</v>
       </c>
@@ -29815,69 +29812,69 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="154" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="96" t="str">
+      <c r="C15" s="155"/>
+      <c r="D15" s="155"/>
+      <c r="E15" s="156"/>
+      <c r="F15" s="130" t="str">
         <f>VLOOKUP(K3,Dados!A:H,5,0)</f>
         <v>35 a 50 psi</v>
       </c>
-      <c r="G15" s="97"/>
-      <c r="H15" s="98"/>
-      <c r="I15" s="103" t="s">
+      <c r="G15" s="157"/>
+      <c r="H15" s="131"/>
+      <c r="I15" s="126" t="s">
         <v>121</v>
       </c>
-      <c r="J15" s="103"/>
-      <c r="K15" s="103" t="s">
+      <c r="J15" s="126"/>
+      <c r="K15" s="126" t="s">
         <v>122</v>
       </c>
-      <c r="L15" s="103"/>
+      <c r="L15" s="126"/>
     </row>
     <row r="16" spans="1:14" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="93" t="s">
+      <c r="B16" s="154" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="94"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="94"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="94"/>
-      <c r="I16" s="100"/>
-      <c r="J16" s="100"/>
-      <c r="K16" s="100"/>
-      <c r="L16" s="101"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="160"/>
     </row>
     <row r="17" spans="2:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="99"/>
-      <c r="C17" s="100"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="100"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="100"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="182" t="s">
+      <c r="B17" s="158"/>
+      <c r="C17" s="159"/>
+      <c r="D17" s="159"/>
+      <c r="E17" s="159"/>
+      <c r="F17" s="159"/>
+      <c r="G17" s="159"/>
+      <c r="H17" s="159"/>
+      <c r="I17" s="178" t="s">
         <v>187</v>
       </c>
-      <c r="J17" s="183"/>
-      <c r="K17" s="182" t="s">
+      <c r="J17" s="179"/>
+      <c r="K17" s="178" t="s">
         <v>187</v>
       </c>
-      <c r="L17" s="183"/>
+      <c r="L17" s="179"/>
     </row>
     <row r="18" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="174" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="126"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="126"/>
-      <c r="F18" s="126"/>
-      <c r="G18" s="126"/>
-      <c r="H18" s="166"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="108"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="108"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="181"/>
       <c r="I18" s="39" t="s">
         <v>2</v>
       </c>
@@ -29892,20 +29889,20 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="153" t="s">
+      <c r="B19" s="97" t="s">
         <v>188</v>
       </c>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
       <c r="F19" s="65" t="str">
         <f>VLOOKUP(K3,Dados!A:AF,5,0)</f>
         <v>35 a 50 psi</v>
       </c>
-      <c r="G19" s="92" t="s">
+      <c r="G19" s="96" t="s">
         <v>125</v>
       </c>
-      <c r="H19" s="176"/>
+      <c r="H19" s="169"/>
       <c r="I19" s="54" t="str">
         <f>VLOOKUP(K3,Dados!A:N,14,0)</f>
         <v>____:____</v>
@@ -29924,10 +29921,10 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="167" t="s">
+      <c r="B20" s="182" t="s">
         <v>189</v>
       </c>
-      <c r="C20" s="155"/>
+      <c r="C20" s="99"/>
       <c r="D20" s="67">
         <f>VLOOKUP(K3,Dados!A:O,12,0)</f>
         <v>1</v>
@@ -29939,10 +29936,10 @@
         <f>VLOOKUP(K3,Dados!A:M,13,0)</f>
         <v>N/A</v>
       </c>
-      <c r="G20" s="155" t="s">
+      <c r="G20" s="99" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="191"/>
+      <c r="H20" s="170"/>
       <c r="I20" s="53" t="str">
         <f>VLOOKUP(K3,Dados!A:P,16,0)</f>
         <v>N/A</v>
@@ -29961,58 +29958,58 @@
       </c>
     </row>
     <row r="21" spans="2:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="171" t="s">
+      <c r="B21" s="186" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="172"/>
-      <c r="D21" s="172"/>
-      <c r="E21" s="172"/>
-      <c r="F21" s="126" t="str">
+      <c r="C21" s="187"/>
+      <c r="D21" s="187"/>
+      <c r="E21" s="187"/>
+      <c r="F21" s="108" t="str">
         <f>VLOOKUP(K3,Dados!A:L,6,0)</f>
         <v>15 min./ Mínimo</v>
       </c>
-      <c r="G21" s="126"/>
-      <c r="H21" s="173"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="175"/>
       <c r="I21" s="61"/>
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="63"/>
     </row>
     <row r="22" spans="2:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="174" t="s">
+      <c r="B22" s="188" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="175"/>
-      <c r="D22" s="175"/>
-      <c r="E22" s="175"/>
-      <c r="F22" s="92" t="str">
+      <c r="C22" s="189"/>
+      <c r="D22" s="189"/>
+      <c r="E22" s="189"/>
+      <c r="F22" s="96" t="str">
         <f>VLOOKUP(K3,Dados!A:H,8,0)</f>
         <v>120 min./ Mínimo</v>
       </c>
-      <c r="G22" s="92"/>
-      <c r="H22" s="176"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="169"/>
       <c r="I22" s="52"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="64"/>
     </row>
     <row r="23" spans="2:12" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="177" t="s">
+      <c r="B23" s="190" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="178"/>
-      <c r="D23" s="178"/>
-      <c r="E23" s="178"/>
-      <c r="F23" s="152" t="str">
+      <c r="C23" s="191"/>
+      <c r="D23" s="191"/>
+      <c r="E23" s="191"/>
+      <c r="F23" s="95" t="str">
         <f>VLOOKUP(K3,Dados!A:J,7,0)</f>
         <v>60ºC</v>
       </c>
-      <c r="G23" s="152"/>
-      <c r="H23" s="168"/>
-      <c r="I23" s="187"/>
-      <c r="J23" s="188"/>
-      <c r="K23" s="189"/>
-      <c r="L23" s="190"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="183"/>
+      <c r="I23" s="165"/>
+      <c r="J23" s="166"/>
+      <c r="K23" s="167"/>
+      <c r="L23" s="168"/>
     </row>
     <row r="24" spans="2:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="48"/>
@@ -30028,32 +30025,32 @@
       <c r="L24" s="51"/>
     </row>
     <row r="25" spans="2:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="186"/>
-      <c r="C25" s="186"/>
-      <c r="D25" s="186"/>
-      <c r="E25" s="186"/>
+      <c r="B25" s="173"/>
+      <c r="C25" s="173"/>
+      <c r="D25" s="173"/>
+      <c r="E25" s="173"/>
       <c r="F25" s="50"/>
-      <c r="G25" s="186"/>
-      <c r="H25" s="186"/>
-      <c r="I25" s="184" t="s">
+      <c r="G25" s="173"/>
+      <c r="H25" s="173"/>
+      <c r="I25" s="171" t="s">
         <v>191</v>
       </c>
-      <c r="J25" s="185"/>
-      <c r="K25" s="184" t="s">
+      <c r="J25" s="172"/>
+      <c r="K25" s="171" t="s">
         <v>191</v>
       </c>
-      <c r="L25" s="185"/>
+      <c r="L25" s="172"/>
     </row>
     <row r="26" spans="2:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="165" t="s">
+      <c r="B26" s="174" t="s">
         <v>124</v>
       </c>
-      <c r="C26" s="126"/>
-      <c r="D26" s="126"/>
-      <c r="E26" s="126"/>
-      <c r="F26" s="126"/>
-      <c r="G26" s="126"/>
-      <c r="H26" s="173"/>
+      <c r="C26" s="108"/>
+      <c r="D26" s="108"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="108"/>
+      <c r="G26" s="108"/>
+      <c r="H26" s="175"/>
       <c r="I26" s="59" t="s">
         <v>2</v>
       </c>
@@ -30068,20 +30065,20 @@
       </c>
     </row>
     <row r="27" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="153" t="s">
+      <c r="B27" s="97" t="s">
         <v>188</v>
       </c>
-      <c r="C27" s="92"/>
-      <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="96"/>
+      <c r="E27" s="96"/>
       <c r="F27" s="72">
         <f>VLOOKUP(K3,Dados!A:Y,25,0)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="162" t="s">
+      <c r="G27" s="192" t="s">
         <v>125</v>
       </c>
-      <c r="H27" s="163"/>
+      <c r="H27" s="193"/>
       <c r="I27" s="61">
         <f>VLOOKUP(K3,Dados!A:AE,26,0)</f>
         <v>0</v>
@@ -30100,10 +30097,10 @@
       </c>
     </row>
     <row r="28" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="164" t="s">
+      <c r="B28" s="194" t="s">
         <v>189</v>
       </c>
-      <c r="C28" s="157"/>
+      <c r="C28" s="101"/>
       <c r="D28" s="73">
         <f>VLOOKUP(K3,Dados!A:AE,31,0)</f>
         <v>0</v>
@@ -30115,10 +30112,10 @@
         <f>VLOOKUP(K3,Dados!A:AF,24,0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="152" t="s">
+      <c r="G28" s="95" t="s">
         <v>126</v>
       </c>
-      <c r="H28" s="168"/>
+      <c r="H28" s="183"/>
       <c r="I28" s="53" t="str">
         <f>VLOOKUP(K3,Dados!A:T,20,0)</f>
         <v>N/A</v>
@@ -30137,139 +30134,139 @@
       </c>
     </row>
     <row r="29" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="105" t="s">
+      <c r="B29" s="163" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="106"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="169" t="str">
+      <c r="C29" s="164"/>
+      <c r="D29" s="164"/>
+      <c r="E29" s="164"/>
+      <c r="F29" s="184" t="str">
         <f>VLOOKUP(K3,Dados!A:H,6,0)</f>
         <v>15 min./ Mínimo</v>
       </c>
-      <c r="G29" s="169"/>
-      <c r="H29" s="170"/>
+      <c r="G29" s="184"/>
+      <c r="H29" s="185"/>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
       <c r="K29" s="27"/>
       <c r="L29" s="28"/>
     </row>
     <row r="30" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="93" t="s">
+      <c r="B30" s="154" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="94"/>
-      <c r="F30" s="97" t="str">
+      <c r="C30" s="155"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="157" t="str">
         <f>VLOOKUP(K3,Dados!A:H,8,0)</f>
         <v>120 min./ Mínimo</v>
       </c>
-      <c r="G30" s="97"/>
-      <c r="H30" s="98"/>
+      <c r="G30" s="157"/>
+      <c r="H30" s="131"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="93" t="s">
+      <c r="B31" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="94"/>
-      <c r="D31" s="94"/>
-      <c r="E31" s="94"/>
-      <c r="F31" s="97" t="str">
+      <c r="C31" s="155"/>
+      <c r="D31" s="155"/>
+      <c r="E31" s="155"/>
+      <c r="F31" s="157" t="str">
         <f>VLOOKUP(K3,Dados!A:H,7,0)</f>
         <v>60ºC</v>
       </c>
-      <c r="G31" s="97"/>
-      <c r="H31" s="98"/>
-      <c r="I31" s="107"/>
-      <c r="J31" s="107"/>
-      <c r="K31" s="91"/>
-      <c r="L31" s="91"/>
+      <c r="G31" s="157"/>
+      <c r="H31" s="131"/>
+      <c r="I31" s="132"/>
+      <c r="J31" s="132"/>
+      <c r="K31" s="153"/>
+      <c r="L31" s="153"/>
     </row>
     <row r="32" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B33" s="108" t="s">
+      <c r="B33" s="133" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="109"/>
-      <c r="D33" s="109"/>
-      <c r="E33" s="109"/>
-      <c r="F33" s="109"/>
-      <c r="G33" s="109"/>
-      <c r="H33" s="109"/>
-      <c r="I33" s="109"/>
-      <c r="J33" s="109"/>
-      <c r="K33" s="109"/>
-      <c r="L33" s="110"/>
+      <c r="C33" s="134"/>
+      <c r="D33" s="134"/>
+      <c r="E33" s="134"/>
+      <c r="F33" s="134"/>
+      <c r="G33" s="134"/>
+      <c r="H33" s="134"/>
+      <c r="I33" s="134"/>
+      <c r="J33" s="134"/>
+      <c r="K33" s="134"/>
+      <c r="L33" s="135"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B34" s="111"/>
-      <c r="C34" s="112"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="112"/>
-      <c r="G34" s="112"/>
-      <c r="H34" s="112"/>
-      <c r="I34" s="112"/>
-      <c r="J34" s="112"/>
-      <c r="K34" s="112"/>
-      <c r="L34" s="113"/>
+      <c r="B34" s="136"/>
+      <c r="C34" s="125"/>
+      <c r="D34" s="125"/>
+      <c r="E34" s="125"/>
+      <c r="F34" s="125"/>
+      <c r="G34" s="125"/>
+      <c r="H34" s="125"/>
+      <c r="I34" s="125"/>
+      <c r="J34" s="125"/>
+      <c r="K34" s="125"/>
+      <c r="L34" s="137"/>
     </row>
     <row r="35" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="117" t="s">
+      <c r="B35" s="141" t="s">
         <v>155</v>
       </c>
-      <c r="C35" s="118"/>
-      <c r="D35" s="118"/>
-      <c r="E35" s="118"/>
-      <c r="F35" s="118"/>
-      <c r="G35" s="118"/>
-      <c r="H35" s="118"/>
-      <c r="I35" s="118" t="s">
+      <c r="C35" s="142"/>
+      <c r="D35" s="142"/>
+      <c r="E35" s="142"/>
+      <c r="F35" s="142"/>
+      <c r="G35" s="142"/>
+      <c r="H35" s="142"/>
+      <c r="I35" s="142" t="s">
         <v>117</v>
       </c>
-      <c r="J35" s="118"/>
-      <c r="K35" s="118"/>
-      <c r="L35" s="119"/>
+      <c r="J35" s="142"/>
+      <c r="K35" s="142"/>
+      <c r="L35" s="143"/>
     </row>
     <row r="36" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="114" t="s">
+      <c r="B36" s="138" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="115"/>
-      <c r="D36" s="115"/>
-      <c r="E36" s="115"/>
-      <c r="F36" s="115"/>
-      <c r="G36" s="115"/>
-      <c r="H36" s="115"/>
-      <c r="I36" s="115" t="s">
+      <c r="C36" s="139"/>
+      <c r="D36" s="139"/>
+      <c r="E36" s="139"/>
+      <c r="F36" s="139"/>
+      <c r="G36" s="139"/>
+      <c r="H36" s="139"/>
+      <c r="I36" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="J36" s="115"/>
-      <c r="K36" s="115"/>
-      <c r="L36" s="116"/>
+      <c r="J36" s="139"/>
+      <c r="K36" s="139"/>
+      <c r="L36" s="140"/>
     </row>
     <row r="37" spans="1:16" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="14"/>
     </row>
     <row r="38" spans="1:16" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="120" t="s">
+      <c r="B38" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="121"/>
-      <c r="D38" s="121"/>
-      <c r="E38" s="121"/>
-      <c r="F38" s="121"/>
-      <c r="G38" s="121"/>
-      <c r="H38" s="121"/>
-      <c r="I38" s="121"/>
-      <c r="J38" s="121"/>
-      <c r="K38" s="121"/>
-      <c r="L38" s="122"/>
+      <c r="C38" s="145"/>
+      <c r="D38" s="145"/>
+      <c r="E38" s="145"/>
+      <c r="F38" s="145"/>
+      <c r="G38" s="145"/>
+      <c r="H38" s="145"/>
+      <c r="I38" s="145"/>
+      <c r="J38" s="145"/>
+      <c r="K38" s="145"/>
+      <c r="L38" s="146"/>
       <c r="P38" t="s">
         <v>16</v>
       </c>
@@ -30284,17 +30281,17 @@
       <c r="B41" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="123" t="s">
+      <c r="C41" s="147" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="124"/>
-      <c r="E41" s="124"/>
-      <c r="F41" s="125"/>
-      <c r="G41" s="104" t="s">
+      <c r="D41" s="148"/>
+      <c r="E41" s="148"/>
+      <c r="F41" s="149"/>
+      <c r="G41" s="162" t="s">
         <v>9</v>
       </c>
-      <c r="H41" s="104"/>
-      <c r="I41" s="104"/>
+      <c r="H41" s="162"/>
+      <c r="I41" s="162"/>
       <c r="J41" s="9" t="s">
         <v>10</v>
       </c>
@@ -30310,17 +30307,17 @@
       <c r="B43" s="5">
         <v>1</v>
       </c>
-      <c r="C43" s="88" t="s">
+      <c r="C43" s="150" t="s">
         <v>230</v>
       </c>
-      <c r="D43" s="89"/>
-      <c r="E43" s="89"/>
-      <c r="F43" s="90"/>
-      <c r="G43" s="160" t="s">
+      <c r="D43" s="151"/>
+      <c r="E43" s="151"/>
+      <c r="F43" s="152"/>
+      <c r="G43" s="195" t="s">
         <v>229</v>
       </c>
-      <c r="H43" s="160"/>
-      <c r="I43" s="160"/>
+      <c r="H43" s="195"/>
+      <c r="I43" s="195"/>
       <c r="J43" s="5">
         <v>5</v>
       </c>
@@ -30333,13 +30330,13 @@
       <c r="B44" s="5">
         <v>2</v>
       </c>
-      <c r="C44" s="88"/>
-      <c r="D44" s="89"/>
-      <c r="E44" s="89"/>
-      <c r="F44" s="90"/>
-      <c r="G44" s="160"/>
-      <c r="H44" s="160"/>
-      <c r="I44" s="160"/>
+      <c r="C44" s="150"/>
+      <c r="D44" s="151"/>
+      <c r="E44" s="151"/>
+      <c r="F44" s="152"/>
+      <c r="G44" s="195"/>
+      <c r="H44" s="195"/>
+      <c r="I44" s="195"/>
       <c r="J44" s="5"/>
       <c r="K44" s="8" t="s">
         <v>118</v>
@@ -30350,13 +30347,13 @@
       <c r="B45" s="5">
         <v>3</v>
       </c>
-      <c r="C45" s="88"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="90"/>
-      <c r="G45" s="160"/>
-      <c r="H45" s="160"/>
-      <c r="I45" s="160"/>
+      <c r="C45" s="150"/>
+      <c r="D45" s="151"/>
+      <c r="E45" s="151"/>
+      <c r="F45" s="152"/>
+      <c r="G45" s="195"/>
+      <c r="H45" s="195"/>
+      <c r="I45" s="195"/>
       <c r="J45" s="5"/>
       <c r="K45" s="8" t="s">
         <v>118</v>
@@ -30367,13 +30364,13 @@
       <c r="B46" s="5">
         <v>4</v>
       </c>
-      <c r="C46" s="88"/>
-      <c r="D46" s="89"/>
-      <c r="E46" s="89"/>
-      <c r="F46" s="90"/>
-      <c r="G46" s="160"/>
-      <c r="H46" s="160"/>
-      <c r="I46" s="160"/>
+      <c r="C46" s="150"/>
+      <c r="D46" s="151"/>
+      <c r="E46" s="151"/>
+      <c r="F46" s="152"/>
+      <c r="G46" s="195"/>
+      <c r="H46" s="195"/>
+      <c r="I46" s="195"/>
       <c r="J46" s="5"/>
       <c r="K46" s="8" t="s">
         <v>118</v>
@@ -30384,13 +30381,13 @@
       <c r="B47" s="5">
         <v>5</v>
       </c>
-      <c r="C47" s="88"/>
-      <c r="D47" s="89"/>
-      <c r="E47" s="89"/>
-      <c r="F47" s="90"/>
-      <c r="G47" s="160"/>
-      <c r="H47" s="160"/>
-      <c r="I47" s="160"/>
+      <c r="C47" s="150"/>
+      <c r="D47" s="151"/>
+      <c r="E47" s="151"/>
+      <c r="F47" s="152"/>
+      <c r="G47" s="195"/>
+      <c r="H47" s="195"/>
+      <c r="I47" s="195"/>
       <c r="J47" s="5"/>
       <c r="K47" s="8" t="s">
         <v>118</v>
@@ -30401,13 +30398,13 @@
       <c r="B48" s="5">
         <v>6</v>
       </c>
-      <c r="C48" s="88"/>
-      <c r="D48" s="89"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="90"/>
-      <c r="G48" s="160"/>
-      <c r="H48" s="160"/>
-      <c r="I48" s="160"/>
+      <c r="C48" s="150"/>
+      <c r="D48" s="151"/>
+      <c r="E48" s="151"/>
+      <c r="F48" s="152"/>
+      <c r="G48" s="195"/>
+      <c r="H48" s="195"/>
+      <c r="I48" s="195"/>
       <c r="J48" s="5"/>
       <c r="K48" s="8" t="s">
         <v>118</v>
@@ -30418,13 +30415,13 @@
       <c r="B49" s="5">
         <v>7</v>
       </c>
-      <c r="C49" s="88"/>
-      <c r="D49" s="89"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="90"/>
-      <c r="G49" s="160"/>
-      <c r="H49" s="160"/>
-      <c r="I49" s="160"/>
+      <c r="C49" s="150"/>
+      <c r="D49" s="151"/>
+      <c r="E49" s="151"/>
+      <c r="F49" s="152"/>
+      <c r="G49" s="195"/>
+      <c r="H49" s="195"/>
+      <c r="I49" s="195"/>
       <c r="J49" s="5"/>
       <c r="K49" s="8" t="s">
         <v>118</v>
@@ -30435,13 +30432,13 @@
       <c r="B50" s="5">
         <v>8</v>
       </c>
-      <c r="C50" s="88"/>
-      <c r="D50" s="89"/>
-      <c r="E50" s="89"/>
-      <c r="F50" s="90"/>
-      <c r="G50" s="160"/>
-      <c r="H50" s="160"/>
-      <c r="I50" s="160"/>
+      <c r="C50" s="150"/>
+      <c r="D50" s="151"/>
+      <c r="E50" s="151"/>
+      <c r="F50" s="152"/>
+      <c r="G50" s="195"/>
+      <c r="H50" s="195"/>
+      <c r="I50" s="195"/>
       <c r="J50" s="6"/>
       <c r="K50" s="8" t="s">
         <v>118</v>
@@ -30452,13 +30449,13 @@
       <c r="B51" s="5">
         <v>9</v>
       </c>
-      <c r="C51" s="88"/>
-      <c r="D51" s="89"/>
-      <c r="E51" s="89"/>
-      <c r="F51" s="90"/>
-      <c r="G51" s="160"/>
-      <c r="H51" s="160"/>
-      <c r="I51" s="160"/>
+      <c r="C51" s="150"/>
+      <c r="D51" s="151"/>
+      <c r="E51" s="151"/>
+      <c r="F51" s="152"/>
+      <c r="G51" s="195"/>
+      <c r="H51" s="195"/>
+      <c r="I51" s="195"/>
       <c r="J51" s="6"/>
       <c r="K51" s="8" t="s">
         <v>118</v>
@@ -30469,13 +30466,13 @@
       <c r="B52" s="5">
         <v>10</v>
       </c>
-      <c r="C52" s="88"/>
-      <c r="D52" s="89"/>
-      <c r="E52" s="89"/>
-      <c r="F52" s="90"/>
-      <c r="G52" s="160"/>
-      <c r="H52" s="160"/>
-      <c r="I52" s="160"/>
+      <c r="C52" s="150"/>
+      <c r="D52" s="151"/>
+      <c r="E52" s="151"/>
+      <c r="F52" s="152"/>
+      <c r="G52" s="195"/>
+      <c r="H52" s="195"/>
+      <c r="I52" s="195"/>
       <c r="J52" s="6"/>
       <c r="K52" s="8" t="s">
         <v>118</v>
@@ -30484,84 +30481,84 @@
     </row>
     <row r="53" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="25"/>
-      <c r="C53" s="158"/>
-      <c r="D53" s="158"/>
-      <c r="E53" s="158"/>
-      <c r="F53" s="158"/>
-      <c r="G53" s="158"/>
-      <c r="H53" s="158"/>
-      <c r="I53" s="158"/>
+      <c r="C53" s="105"/>
+      <c r="D53" s="105"/>
+      <c r="E53" s="105"/>
+      <c r="F53" s="105"/>
+      <c r="G53" s="105"/>
+      <c r="H53" s="105"/>
+      <c r="I53" s="105"/>
       <c r="K53" s="7"/>
       <c r="L53" s="25"/>
     </row>
     <row r="54" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="159" t="s">
+      <c r="B54" s="106" t="s">
         <v>120</v>
       </c>
-      <c r="C54" s="159"/>
-      <c r="D54" s="159"/>
-      <c r="E54" s="159"/>
-      <c r="F54" s="159"/>
-      <c r="G54" s="159"/>
-      <c r="H54" s="159"/>
-      <c r="I54" s="159"/>
-      <c r="J54" s="159"/>
-      <c r="K54" s="159"/>
-      <c r="L54" s="159"/>
+      <c r="C54" s="106"/>
+      <c r="D54" s="106"/>
+      <c r="E54" s="106"/>
+      <c r="F54" s="106"/>
+      <c r="G54" s="106"/>
+      <c r="H54" s="106"/>
+      <c r="I54" s="106"/>
+      <c r="J54" s="106"/>
+      <c r="K54" s="106"/>
+      <c r="L54" s="106"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B56" s="161" t="s">
+      <c r="B56" s="196" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="161"/>
-      <c r="D56" s="161"/>
-      <c r="E56" s="161"/>
-      <c r="F56" s="161"/>
-      <c r="G56" s="161"/>
-      <c r="H56" s="161"/>
-      <c r="I56" s="161"/>
-      <c r="J56" s="161"/>
-      <c r="K56" s="161"/>
-      <c r="L56" s="161"/>
+      <c r="C56" s="196"/>
+      <c r="D56" s="196"/>
+      <c r="E56" s="196"/>
+      <c r="F56" s="196"/>
+      <c r="G56" s="196"/>
+      <c r="H56" s="196"/>
+      <c r="I56" s="196"/>
+      <c r="J56" s="196"/>
+      <c r="K56" s="196"/>
+      <c r="L56" s="196"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B57" s="161"/>
-      <c r="C57" s="161"/>
-      <c r="D57" s="161"/>
-      <c r="E57" s="161"/>
-      <c r="F57" s="161"/>
-      <c r="G57" s="161"/>
-      <c r="H57" s="161"/>
-      <c r="I57" s="161"/>
-      <c r="J57" s="161"/>
-      <c r="K57" s="161"/>
-      <c r="L57" s="161"/>
+      <c r="B57" s="196"/>
+      <c r="C57" s="196"/>
+      <c r="D57" s="196"/>
+      <c r="E57" s="196"/>
+      <c r="F57" s="196"/>
+      <c r="G57" s="196"/>
+      <c r="H57" s="196"/>
+      <c r="I57" s="196"/>
+      <c r="J57" s="196"/>
+      <c r="K57" s="196"/>
+      <c r="L57" s="196"/>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B58" s="161"/>
-      <c r="C58" s="161"/>
-      <c r="D58" s="161"/>
-      <c r="E58" s="161"/>
-      <c r="F58" s="161"/>
-      <c r="G58" s="161"/>
-      <c r="H58" s="161"/>
-      <c r="I58" s="161"/>
-      <c r="J58" s="161"/>
-      <c r="K58" s="161"/>
-      <c r="L58" s="161"/>
+      <c r="B58" s="196"/>
+      <c r="C58" s="196"/>
+      <c r="D58" s="196"/>
+      <c r="E58" s="196"/>
+      <c r="F58" s="196"/>
+      <c r="G58" s="196"/>
+      <c r="H58" s="196"/>
+      <c r="I58" s="196"/>
+      <c r="J58" s="196"/>
+      <c r="K58" s="196"/>
+      <c r="L58" s="196"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B59" s="161"/>
-      <c r="C59" s="161"/>
-      <c r="D59" s="161"/>
-      <c r="E59" s="161"/>
-      <c r="F59" s="161"/>
-      <c r="G59" s="161"/>
-      <c r="H59" s="161"/>
-      <c r="I59" s="161"/>
-      <c r="J59" s="161"/>
-      <c r="K59" s="161"/>
-      <c r="L59" s="161"/>
+      <c r="B59" s="196"/>
+      <c r="C59" s="196"/>
+      <c r="D59" s="196"/>
+      <c r="E59" s="196"/>
+      <c r="F59" s="196"/>
+      <c r="G59" s="196"/>
+      <c r="H59" s="196"/>
+      <c r="I59" s="196"/>
+      <c r="J59" s="196"/>
+      <c r="K59" s="196"/>
+      <c r="L59" s="196"/>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
@@ -30573,55 +30570,26 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B6:L7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="B16:L16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B1:L2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="C52:F52"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="B56:L59"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="B54:L54"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="G47:I47"/>
     <mergeCell ref="C44:F44"/>
     <mergeCell ref="G44:I44"/>
     <mergeCell ref="I31:J31"/>
@@ -30638,26 +30606,55 @@
     <mergeCell ref="G41:I41"/>
     <mergeCell ref="C43:F43"/>
     <mergeCell ref="G43:I43"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="C52:F52"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="B56:L59"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="B54:L54"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="B1:L2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B6:L7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="B16:L16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>

</xml_diff>